<commit_message>
funcion para subir plantilla con estudiantes
</commit_message>
<xml_diff>
--- a/public/reportes/informe.xlsx
+++ b/public/reportes/informe.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="182">
   <si>
     <t>INFORME DE VISITAS DIARIAS DE CADA ENTIDAD</t>
   </si>
@@ -544,6 +544,21 @@
   <si>
     <t>2024-06-25</t>
   </si>
+  <si>
+    <t>2024-10-10</t>
+  </si>
+  <si>
+    <t>2024-10-11</t>
+  </si>
+  <si>
+    <t>2024-10-14</t>
+  </si>
+  <si>
+    <t>2024-10-15</t>
+  </si>
+  <si>
+    <t>2024-10-16</t>
+  </si>
 </sst>
 </file>
 
@@ -21159,10 +21174,10 @@
     </row>
     <row r="1835" spans="1:3">
       <c r="A1835" s="4" t="s">
-        <v>86</v>
+        <v>177</v>
       </c>
       <c r="B1835" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="C1835" s="4">
         <v>1</v>
@@ -21170,43 +21185,43 @@
     </row>
     <row r="1836" spans="1:3">
       <c r="A1836" s="4" t="s">
-        <v>86</v>
+        <v>178</v>
       </c>
       <c r="B1836" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="C1836" s="4">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1837" spans="1:3">
       <c r="A1837" s="4" t="s">
-        <v>86</v>
+        <v>179</v>
       </c>
       <c r="B1837" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="C1837" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1838" spans="1:3">
       <c r="A1838" s="4" t="s">
-        <v>86</v>
+        <v>180</v>
       </c>
       <c r="B1838" t="s">
-        <v>15</v>
+        <v>102</v>
       </c>
       <c r="C1838" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1839" spans="1:3">
       <c r="A1839" s="4" t="s">
-        <v>86</v>
+        <v>181</v>
       </c>
       <c r="B1839" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="C1839" s="4">
         <v>1</v>
@@ -70895,5 +70910,14 @@
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>